<commit_message>
add Power BI file
</commit_message>
<xml_diff>
--- a/Report/Amazon Sales Report.xlsx
+++ b/Report/Amazon Sales Report.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Amazon Sale Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5831C16B-C6DC-469F-BBF0-C9800C6AA171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD94073-A2AA-4A45-B694-6C3EBF0F9CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{1DE24626-BF60-4871-8242-B0FFC979D36A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{1DE24626-BF60-4871-8242-B0FFC979D36A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="KYV - Column" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Cleaning" sheetId="2" r:id="rId2"/>
+    <sheet name="Data-Transformation-Wrangling" sheetId="3" r:id="rId3"/>
+    <sheet name="StoryTelling KPI-Charts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,9 +36,203 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+  <si>
+    <t>Know Your Value/Column</t>
+  </si>
+  <si>
+    <t>Befor Transformation</t>
+  </si>
+  <si>
+    <t>After Transformation</t>
+  </si>
+  <si>
+    <t>Col No.</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Description / Purpose</t>
+  </si>
+  <si>
+    <t>KYD Data Cleaning</t>
+  </si>
+  <si>
+    <t>Sr. No.</t>
+  </si>
+  <si>
+    <t>Applied Steps</t>
+  </si>
+  <si>
+    <t>Rows Before</t>
+  </si>
+  <si>
+    <t>Rows After</t>
+  </si>
+  <si>
+    <t>Effect (Rows)</t>
+  </si>
+  <si>
+    <t>Col Before</t>
+  </si>
+  <si>
+    <t>Col After</t>
+  </si>
+  <si>
+    <t>Effect (Columns)</t>
+  </si>
+  <si>
+    <t>Data-Transformation-Wrangling</t>
+  </si>
+  <si>
+    <t>Performed Activity (Data Wrangling Step)</t>
+  </si>
+  <si>
+    <t>Story Telling KPI's &amp; Charts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Dashboard </t>
+  </si>
+  <si>
+    <t>KPI's</t>
+  </si>
+  <si>
+    <t>Visuals</t>
+  </si>
+  <si>
+    <t>Filters / Slicers</t>
+  </si>
+  <si>
+    <t>KPI's Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Chart Name</t>
+  </si>
+  <si>
+    <t>Columns Used</t>
+  </si>
+  <si>
+    <t>Visual Type</t>
+  </si>
+  <si>
+    <t>Insight / Purpose</t>
+  </si>
+  <si>
+    <t>Filter / Slicer Name</t>
+  </si>
+  <si>
+    <t>Used Column</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Fulfilment</t>
+  </si>
+  <si>
+    <t>Sales Channel</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Fulfilled By</t>
+  </si>
+  <si>
+    <t>Unique order number</t>
+  </si>
+  <si>
+    <t>Order placed date</t>
+  </si>
+  <si>
+    <t>Current status (Delivered / Cancelled / Shipped)</t>
+  </si>
+  <si>
+    <t>Who fulfilled the order</t>
+  </si>
+  <si>
+    <t>Amazon.in</t>
+  </si>
+  <si>
+    <t>Shipping Type</t>
+  </si>
+  <si>
+    <t>Standard / Expedited</t>
+  </si>
+  <si>
+    <t>Product category</t>
+  </si>
+  <si>
+    <t>Product size</t>
+  </si>
+  <si>
+    <t>Quantity ordered</t>
+  </si>
+  <si>
+    <t>Total sale amount</t>
+  </si>
+  <si>
+    <t>Shipping city</t>
+  </si>
+  <si>
+    <t>Shipping state</t>
+  </si>
+  <si>
+    <t>Shipping country</t>
+  </si>
+  <si>
+    <t>Easy Ship / Amazon / Merchant</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Derived year column</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Derived month column</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -46,16 +240,131 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Emoji"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Segoe UI Emoji"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,12 +372,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,48 +760,514 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B3E6E2D-EEAD-4E4A-8798-C3B53E352FF0}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="21" x14ac:dyDescent="0.4">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>8</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>11</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>12</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>14</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>15</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>16</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B6ADD15-B19C-416D-8A8B-7194E6C0A6D6}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:K16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:11" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D12" s="19"/>
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D13" s="19"/>
+      <c r="E13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7AAEBDA-2918-4347-B5CD-94210A58680A}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="D3" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F4FDCB3-6CAE-4927-8D50-CB20F0599746}">
-  <dimension ref="A1"/>
+  <dimension ref="B3:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="17.21875" customWidth="1"/>
+    <col min="14" max="14" width="17" customWidth="1"/>
+    <col min="16" max="16" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.88671875" customWidth="1"/>
+    <col min="19" max="19" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:19" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+    </row>
+    <row r="5" spans="2:19" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+    </row>
+    <row r="7" spans="2:19" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Make Plan for Dashboard & Home ➜ Overview ➜ Product ➜ Fulfilment ➜ Regional ➜ Promotion ➜ (Forecasting Optional)
</commit_message>
<xml_diff>
--- a/Report/Amazon Sales Report.xlsx
+++ b/Report/Amazon Sales Report.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\BI Amazon Sale Report\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3632587-6E3A-4CC7-98BB-A162D0906F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC446B6-2E32-4894-AFC7-8488DB66EAD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{1DE24626-BF60-4871-8242-B0FFC979D36A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{1DE24626-BF60-4871-8242-B0FFC979D36A}"/>
   </bookViews>
   <sheets>
     <sheet name="KYV - Column" sheetId="1" r:id="rId1"/>
     <sheet name="Data Cleaning" sheetId="2" r:id="rId2"/>
     <sheet name="Data-Transformation-Wrangling" sheetId="3" r:id="rId3"/>
     <sheet name="StoryTelling KPI-Charts" sheetId="4" r:id="rId4"/>
+    <sheet name="Plan" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="163">
   <si>
     <t>Know Your Value/Column</t>
   </si>
@@ -518,6 +519,238 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> — represents total order value</t>
+    </r>
+  </si>
+  <si>
+    <t>Final Dashboard Page Plan</t>
+  </si>
+  <si>
+    <t>Page No.</t>
+  </si>
+  <si>
+    <t>Page Name</t>
+  </si>
+  <si>
+    <t>Purpose / Focus</t>
+  </si>
+  <si>
+    <t>Key Columns Used</t>
+  </si>
+  <si>
+    <t>Example Insights / Visuals</t>
+  </si>
+  <si>
+    <t>Home Page</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Buttons linking to Overview, Product Insights, Fulfilment, Regional, Promotion pages. Add branding, title, and theme.</t>
+  </si>
+  <si>
+    <t>Overview Dashboard</t>
+  </si>
+  <si>
+    <t>Date, Year, Month, Week, Total Amount, Qty, Category, State, Fulfilment, B2B</t>
+  </si>
+  <si>
+    <t>KPIs (Total Sales, Orders, Avg. Order Value), Monthly Trend, Top Category, Fulfilment Share, Region Heatmap, etc.</t>
+  </si>
+  <si>
+    <t>Product Insights</t>
+  </si>
+  <si>
+    <t>Category, Size, SKU, Qty, Total Amount</t>
+  </si>
+  <si>
+    <t>Best-selling categories, Size-wise performance, SKU-level profit, Product demand pattern.</t>
+  </si>
+  <si>
+    <t>Fulfilment &amp; Delivery</t>
+  </si>
+  <si>
+    <t>Fulfilment, Order Type, Fulfilled By, Courier Status, Shipping Type, Status</t>
+  </si>
+  <si>
+    <t>FBA vs FBM comparison, delivery vs cancelled %, courier performance.</t>
+  </si>
+  <si>
+    <t>Regional Analysis</t>
+  </si>
+  <si>
+    <t>City, State, Country, Total Amount, Qty</t>
+  </si>
+  <si>
+    <t>State-wise map, top 10 cities, sales heatmap, regional contribution %.</t>
+  </si>
+  <si>
+    <t>Promotion &amp; Revenue Analysis</t>
+  </si>
+  <si>
+    <t>Promotion IDs, B2B, Total Amount, Qty, Date</t>
+  </si>
+  <si>
+    <t>Impact of promotions on sales, B2B vs B2C ratio, average revenue per order.</t>
+  </si>
+  <si>
+    <t>7 (Optional)</t>
+  </si>
+  <si>
+    <t>Trend &amp; Forecasting (Advanced)</t>
+  </si>
+  <si>
+    <t>Predict future sales and show time-based patterns.</t>
+  </si>
+  <si>
+    <t>Date, Total Amount, Qty</t>
+  </si>
+  <si>
+    <t>Monthly trends, seasonality, sales forecast using Power BI Analytics pane.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Acts as the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>main navigation hub</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; only contains buttons (no visuals/slicers).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>High-level summary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — contains 1 key visual from each section + buttons to open detailed pages.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Focus on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>what products drive performance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Focus on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>who fulfilled orders and shipping performance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Focus on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>where sales are coming from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Focus on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>offers, B2B orders, and revenue patterns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
     </r>
   </si>
 </sst>
@@ -624,7 +857,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,6 +912,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -707,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -776,14 +1015,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1163,10 +1408,10 @@
       <c r="F7" s="22">
         <v>1</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="27" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1183,10 +1428,10 @@
       <c r="F8" s="22">
         <v>2</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="27" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1203,10 +1448,10 @@
       <c r="F9" s="22">
         <v>3</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="H9" s="27" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1223,10 +1468,10 @@
       <c r="F10" s="22">
         <v>4</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="27" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1243,10 +1488,10 @@
       <c r="F11" s="22">
         <v>5</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="27" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1263,10 +1508,10 @@
       <c r="F12" s="22">
         <v>6</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="29" t="s">
+      <c r="H12" s="27" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1283,10 +1528,10 @@
       <c r="F13" s="22">
         <v>7</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="27" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1303,10 +1548,10 @@
       <c r="F14" s="22">
         <v>8</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="27" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1323,10 +1568,10 @@
       <c r="F15" s="22">
         <v>9</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="27" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1343,10 +1588,10 @@
       <c r="F16" s="22">
         <v>10</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="27" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1363,10 +1608,10 @@
       <c r="F17" s="22">
         <v>11</v>
       </c>
-      <c r="G17" s="28" t="s">
+      <c r="G17" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="29" t="s">
+      <c r="H17" s="27" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1383,10 +1628,10 @@
       <c r="F18" s="22">
         <v>12</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="29" t="s">
+      <c r="H18" s="27" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1403,10 +1648,10 @@
       <c r="F19" s="22">
         <v>13</v>
       </c>
-      <c r="G19" s="28" t="s">
+      <c r="G19" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="29" t="s">
+      <c r="H19" s="27" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1423,10 +1668,10 @@
       <c r="F20" s="22">
         <v>14</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="H20" s="29" t="s">
+      <c r="H20" s="27" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1443,10 +1688,10 @@
       <c r="F21" s="22">
         <v>15</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H21" s="29" t="s">
+      <c r="H21" s="27" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1463,10 +1708,10 @@
       <c r="F22" s="22">
         <v>16</v>
       </c>
-      <c r="G22" s="28" t="s">
+      <c r="G22" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="27" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1483,10 +1728,10 @@
       <c r="F23" s="22">
         <v>17</v>
       </c>
-      <c r="G23" s="28" t="s">
+      <c r="G23" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="29" t="s">
+      <c r="H23" s="27" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1503,10 +1748,10 @@
       <c r="F24" s="22">
         <v>18</v>
       </c>
-      <c r="G24" s="28" t="s">
+      <c r="G24" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="29" t="s">
+      <c r="H24" s="27" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1523,10 +1768,10 @@
       <c r="F25" s="22">
         <v>19</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G25" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="29" t="s">
+      <c r="H25" s="27" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1543,10 +1788,10 @@
       <c r="F26" s="22">
         <v>20</v>
       </c>
-      <c r="G26" s="28" t="s">
+      <c r="G26" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="H26" s="29" t="s">
+      <c r="H26" s="27" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1563,10 +1808,10 @@
       <c r="F27" s="22">
         <v>21</v>
       </c>
-      <c r="G27" s="28" t="s">
+      <c r="G27" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H27" s="27" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1583,10 +1828,10 @@
       <c r="F28" s="22">
         <v>22</v>
       </c>
-      <c r="G28" s="28" t="s">
+      <c r="G28" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="H28" s="27" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2223,101 +2468,101 @@
       </c>
     </row>
     <row r="23" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="26">
+      <c r="B23" s="20">
         <v>17</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D23" t="s">
         <v>125</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="21">
         <v>17</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="21">
         <f>G22</f>
         <v>113698</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="21">
         <v>113698</v>
       </c>
-      <c r="H23" s="27">
+      <c r="H23" s="21">
         <v>0</v>
       </c>
-      <c r="I23" s="27">
+      <c r="I23" s="21">
         <v>25</v>
       </c>
-      <c r="J23" s="27">
+      <c r="J23" s="21">
         <v>24</v>
       </c>
-      <c r="K23" s="27">
+      <c r="K23" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="26">
+      <c r="B24" s="20">
         <v>18</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D24" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E24" s="21">
         <v>18</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="21">
         <f>G23</f>
         <v>113698</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="21">
         <v>113698</v>
       </c>
-      <c r="H24" s="27">
+      <c r="H24" s="21">
         <v>0</v>
       </c>
-      <c r="I24" s="27">
+      <c r="I24" s="21">
         <v>24</v>
       </c>
-      <c r="J24" s="27">
+      <c r="J24" s="21">
         <v>23</v>
       </c>
-      <c r="K24" s="27">
+      <c r="K24" s="21">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B25" s="26">
+      <c r="B25" s="20">
         <v>19</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="20" t="s">
         <v>50</v>
       </c>
       <c r="D25" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="21">
         <v>19</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="21">
         <f>G24</f>
         <v>113698</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="21">
         <v>113698</v>
       </c>
-      <c r="H25" s="27">
+      <c r="H25" s="21">
         <v>0</v>
       </c>
-      <c r="I25" s="27">
+      <c r="I25" s="21">
         <v>13</v>
       </c>
-      <c r="J25" s="27">
+      <c r="J25" s="21">
         <v>22</v>
       </c>
-      <c r="K25" s="27">
+      <c r="K25" s="21">
         <v>1</v>
       </c>
     </row>
@@ -2330,7 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7AAEBDA-2918-4347-B5CD-94210A58680A}">
   <dimension ref="B3:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -2543,4 +2788,168 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D08B4F4-38F3-4EC4-8131-B24327749222}">
+  <dimension ref="B3:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B3" s="29" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C5" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C7" s="28">
+        <v>2</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C8" s="28">
+        <v>3</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C9" s="28">
+        <v>4</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C10" s="28">
+        <v>5</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="C11" s="28">
+        <v>6</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="C12" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>